<commit_message>
arreglos filtros + nuevas modificaciones3
</commit_message>
<xml_diff>
--- a/prueba27/copia_B.06390_FFT_PS_MB_VAN_EA_DF1_Mangueras(2).xlsx
+++ b/prueba27/copia_B.06390_FFT_PS_MB_VAN_EA_DF1_Mangueras(2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enkro\P00106-ENKROSS_PRUEBA3_AUTOMATIZACION\prueba27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343B9280-408F-4252-AC6F-49E6839758D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11322FC5-CDF5-4504-A6EB-51984B54A7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7075,8 +7075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R292"/>
   <sheetViews>
-    <sheetView topLeftCell="G255" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H292" sqref="H292"/>
+    <sheetView topLeftCell="A255" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G272" sqref="G272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20853,18 +20853,18 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:B4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="59.109375" style="4" customWidth="1"/>
     <col min="4" max="8" width="23.21875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>793</v>
       </c>
@@ -20875,7 +20875,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>796</v>
       </c>
@@ -20886,7 +20886,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>799</v>
       </c>
@@ -20897,7 +20897,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>801</v>
       </c>
@@ -20908,7 +20908,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>803</v>
       </c>
@@ -20919,7 +20919,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>805</v>
       </c>
@@ -20930,7 +20930,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>808</v>
       </c>
@@ -20941,7 +20941,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>810</v>
       </c>
@@ -20952,7 +20952,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>813</v>
       </c>
@@ -20963,7 +20963,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>816</v>
       </c>
@@ -20974,7 +20974,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>818</v>
       </c>
@@ -20985,7 +20985,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>820</v>
       </c>
@@ -20996,7 +20996,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>822</v>
       </c>
@@ -21007,7 +21007,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>824</v>
       </c>
@@ -21018,7 +21018,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>826</v>
       </c>
@@ -21029,7 +21029,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>828</v>
       </c>
@@ -21040,7 +21040,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>830</v>
       </c>
@@ -21051,7 +21051,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>832</v>
       </c>
@@ -21062,7 +21062,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>834</v>
       </c>
@@ -21082,7 +21082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -21093,7 +21093,7 @@
     <col min="3" max="14" width="29" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>835</v>
       </c>
@@ -21122,7 +21122,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>844</v>
       </c>
@@ -21157,7 +21157,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="165.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>855</v>
       </c>
@@ -21168,7 +21168,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>858</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>861</v>
       </c>
@@ -21190,7 +21190,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>864</v>
       </c>
@@ -21201,7 +21201,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>867</v>
       </c>
@@ -21212,7 +21212,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>870</v>
       </c>
@@ -21223,7 +21223,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>873</v>
       </c>
@@ -21234,7 +21234,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>876</v>
       </c>
@@ -21245,7 +21245,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>879</v>
       </c>
@@ -21262,7 +21262,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>883</v>
       </c>
@@ -21273,7 +21273,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>885</v>
       </c>
@@ -21284,7 +21284,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>888</v>
       </c>
@@ -21307,7 +21307,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>895</v>
       </c>
@@ -21330,7 +21330,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="216" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>902</v>
       </c>
@@ -21341,7 +21341,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>905</v>
       </c>
@@ -21358,7 +21358,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>910</v>
       </c>
@@ -21381,7 +21381,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>917</v>
       </c>
@@ -21404,7 +21404,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>924</v>
       </c>
@@ -21415,7 +21415,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>927</v>
       </c>
@@ -21438,7 +21438,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>934</v>
       </c>
@@ -21449,7 +21449,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>936</v>
       </c>
@@ -21460,7 +21460,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>938</v>
       </c>
@@ -21471,7 +21471,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>938</v>
       </c>
@@ -21482,7 +21482,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>943</v>
       </c>
@@ -21493,7 +21493,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>933</v>
       </c>
@@ -21510,7 +21510,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>933</v>
       </c>
@@ -21521,7 +21521,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>933</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>954</v>
       </c>
@@ -21549,7 +21549,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>959</v>
       </c>
@@ -21560,7 +21560,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>962</v>
       </c>
@@ -21571,7 +21571,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>965</v>
       </c>
@@ -21582,7 +21582,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>968</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>972</v>
       </c>
@@ -21610,7 +21610,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>974</v>
       </c>
@@ -21621,7 +21621,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>977</v>
       </c>
@@ -21638,7 +21638,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>981</v>
       </c>
@@ -21649,7 +21649,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>984</v>
       </c>
@@ -21660,7 +21660,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>987</v>
       </c>
@@ -21671,7 +21671,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>990</v>
       </c>
@@ -21682,7 +21682,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>993</v>
       </c>
@@ -21705,7 +21705,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>1000</v>
       </c>
@@ -21728,7 +21728,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>1007</v>
       </c>
@@ -21739,7 +21739,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>1010</v>
       </c>
@@ -21756,7 +21756,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>1015</v>
       </c>
@@ -21779,7 +21779,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>1022</v>
       </c>
@@ -21802,7 +21802,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>1029</v>
       </c>
@@ -21813,7 +21813,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>1032</v>
       </c>
@@ -21824,7 +21824,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>1035</v>
       </c>
@@ -21835,7 +21835,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>1038</v>
       </c>
@@ -21846,7 +21846,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>1041</v>
       </c>
@@ -21857,7 +21857,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>1044</v>
       </c>
@@ -21874,7 +21874,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>1049</v>
       </c>
@@ -21885,7 +21885,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>1052</v>
       </c>
@@ -21896,7 +21896,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>1055</v>
       </c>
@@ -21907,7 +21907,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>1058</v>
       </c>
@@ -21918,7 +21918,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>1061</v>
       </c>
@@ -21929,7 +21929,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>1064</v>
       </c>
@@ -21946,7 +21946,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>1068</v>
       </c>
@@ -21957,7 +21957,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>1070</v>
       </c>
@@ -21968,7 +21968,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>1073</v>
       </c>
@@ -21979,7 +21979,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>1076</v>
       </c>
@@ -21990,7 +21990,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>1076</v>
       </c>
@@ -22001,7 +22001,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>1081</v>
       </c>
@@ -22018,7 +22018,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>1086</v>
       </c>
@@ -22029,7 +22029,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>947</v>
       </c>
@@ -22040,7 +22040,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>1091</v>
       </c>
@@ -22057,7 +22057,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>1096</v>
       </c>
@@ -22068,7 +22068,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>1099</v>
       </c>
@@ -22079,7 +22079,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>1102</v>
       </c>
@@ -22090,7 +22090,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>1105</v>
       </c>
@@ -22101,7 +22101,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>1108</v>
       </c>
@@ -22118,7 +22118,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>1113</v>
       </c>
@@ -22129,7 +22129,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>1115</v>
       </c>
@@ -22140,7 +22140,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>1118</v>
       </c>
@@ -22163,7 +22163,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>1125</v>
       </c>
@@ -22186,7 +22186,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>1132</v>
       </c>
@@ -22197,7 +22197,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>1135</v>
       </c>
@@ -22214,7 +22214,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>1140</v>
       </c>
@@ -22237,7 +22237,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>1147</v>
       </c>
@@ -22260,7 +22260,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>1154</v>
       </c>
@@ -22271,7 +22271,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>1157</v>
       </c>
@@ -22294,7 +22294,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>1164</v>
       </c>
@@ -22305,7 +22305,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>1166</v>
       </c>
@@ -22316,7 +22316,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>1168</v>
       </c>
@@ -22327,7 +22327,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>1168</v>
       </c>
@@ -22338,7 +22338,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>1173</v>
       </c>
@@ -22349,7 +22349,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>1175</v>
       </c>
@@ -22360,7 +22360,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>1163</v>
       </c>
@@ -22377,7 +22377,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>1163</v>
       </c>
@@ -22388,7 +22388,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>1163</v>
       </c>
@@ -22399,7 +22399,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>1185</v>
       </c>
@@ -22416,7 +22416,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>1190</v>
       </c>
@@ -22427,7 +22427,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>1193</v>
       </c>
@@ -22438,7 +22438,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>1196</v>
       </c>
@@ -22449,7 +22449,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>1199</v>
       </c>
@@ -22472,7 +22472,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>1206</v>
       </c>
@@ -22495,7 +22495,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>1213</v>
       </c>
@@ -22506,7 +22506,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>1216</v>
       </c>
@@ -22523,7 +22523,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>1221</v>
       </c>
@@ -22546,7 +22546,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>1228</v>
       </c>
@@ -22569,7 +22569,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>1235</v>
       </c>
@@ -22580,7 +22580,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>1238</v>
       </c>
@@ -22603,7 +22603,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>1085</v>
       </c>
@@ -22614,7 +22614,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>1178</v>
       </c>
@@ -22625,7 +22625,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>1247</v>
       </c>
@@ -22642,7 +22642,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>1252</v>
       </c>
@@ -22653,7 +22653,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>1255</v>
       </c>
@@ -22664,7 +22664,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>1258</v>
       </c>
@@ -22681,7 +22681,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>1262</v>
       </c>
@@ -22692,7 +22692,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>1265</v>
       </c>
@@ -22703,7 +22703,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>1268</v>
       </c>
@@ -22714,7 +22714,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>1271</v>
       </c>
@@ -22737,7 +22737,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>1278</v>
       </c>
@@ -22760,7 +22760,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>1285</v>
       </c>
@@ -22771,7 +22771,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>1288</v>
       </c>
@@ -22788,7 +22788,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>1293</v>
       </c>
@@ -22811,7 +22811,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>1300</v>
       </c>
@@ -22834,7 +22834,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>1307</v>
       </c>
@@ -22845,7 +22845,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>1310</v>
       </c>
@@ -22868,7 +22868,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>1317</v>
       </c>
@@ -22891,7 +22891,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>1324</v>
       </c>
@@ -22902,7 +22902,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>1327</v>
       </c>
@@ -22919,7 +22919,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>1332</v>
       </c>
@@ -22942,7 +22942,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>1339</v>
       </c>
@@ -22965,7 +22965,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>1346</v>
       </c>
@@ -22976,7 +22976,7 @@
         <v>1348</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>1349</v>
       </c>
@@ -22987,7 +22987,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>1349</v>
       </c>
@@ -22998,7 +22998,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>1354</v>
       </c>
@@ -23009,7 +23009,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>1356</v>
       </c>
@@ -23026,7 +23026,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>1361</v>
       </c>
@@ -23037,7 +23037,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>1364</v>
       </c>
@@ -23048,7 +23048,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>1367</v>
       </c>
@@ -23065,7 +23065,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>1372</v>
       </c>
@@ -23076,7 +23076,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>1375</v>
       </c>
@@ -23087,7 +23087,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>1378</v>
       </c>
@@ -23098,7 +23098,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>1381</v>
       </c>
@@ -23115,7 +23115,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>1386</v>
       </c>
@@ -23132,7 +23132,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>1391</v>
       </c>
@@ -23143,7 +23143,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>1393</v>
       </c>
@@ -23154,7 +23154,7 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>1393</v>
       </c>
@@ -23165,7 +23165,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23176,7 +23176,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23187,7 +23187,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23198,7 +23198,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23209,7 +23209,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23220,7 +23220,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23231,7 +23231,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23242,7 +23242,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23253,7 +23253,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23264,7 +23264,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23275,7 +23275,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23286,7 +23286,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>1398</v>
       </c>
@@ -23297,7 +23297,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>1423</v>
       </c>
@@ -23308,7 +23308,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>1423</v>
       </c>
@@ -23319,7 +23319,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>1423</v>
       </c>
@@ -23330,7 +23330,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>1423</v>
       </c>
@@ -23347,7 +23347,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>1430</v>
       </c>
@@ -23364,7 +23364,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>1430</v>
       </c>
@@ -23375,7 +23375,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>1430</v>
       </c>
@@ -23386,7 +23386,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>1436</v>
       </c>
@@ -23397,7 +23397,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>1436</v>
       </c>
@@ -23408,7 +23408,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>1436</v>
       </c>
@@ -23419,7 +23419,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>1436</v>
       </c>
@@ -23430,7 +23430,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>1441</v>
       </c>
@@ -23441,7 +23441,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>1444</v>
       </c>
@@ -23452,7 +23452,7 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23463,7 +23463,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23474,7 +23474,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23485,7 +23485,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23496,7 +23496,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23507,7 +23507,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23518,7 +23518,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23529,7 +23529,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>1447</v>
       </c>
@@ -23540,7 +23540,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>1461</v>
       </c>
@@ -23551,7 +23551,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>1464</v>
       </c>
@@ -23562,7 +23562,7 @@
         <v>1466</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>1467</v>
       </c>
@@ -23573,7 +23573,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>1470</v>
       </c>
@@ -23584,7 +23584,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>1473</v>
       </c>
@@ -23595,7 +23595,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>1476</v>
       </c>
@@ -23606,7 +23606,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>1479</v>
       </c>
@@ -23617,7 +23617,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
         <v>1482</v>
       </c>
@@ -23628,7 +23628,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
         <v>1485</v>
       </c>
@@ -23639,7 +23639,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
         <v>1488</v>
       </c>
@@ -23650,7 +23650,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>1491</v>
       </c>
@@ -23661,7 +23661,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>1494</v>
       </c>
@@ -23672,7 +23672,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
         <v>1497</v>
       </c>
@@ -23683,7 +23683,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
         <v>1500</v>
       </c>
@@ -23694,7 +23694,7 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>1503</v>
       </c>
@@ -23705,7 +23705,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>1506</v>
       </c>
@@ -23716,7 +23716,7 @@
         <v>1508</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>1509</v>
       </c>
@@ -23727,7 +23727,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>1512</v>
       </c>
@@ -23738,7 +23738,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>1515</v>
       </c>
@@ -23749,7 +23749,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>1518</v>
       </c>
@@ -23760,7 +23760,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>1393</v>
       </c>
@@ -23771,7 +23771,7 @@
         <v>1522</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>1430</v>
       </c>
@@ -23782,7 +23782,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>1524</v>
       </c>
@@ -23793,7 +23793,7 @@
         <v>1526</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>1524</v>
       </c>
@@ -23804,7 +23804,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
         <v>1524</v>
       </c>

</xml_diff>